<commit_message>
GHG files from google drive
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Raw_GHG/2020/Raw/GC 30jun20.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Raw_GHG/2020/Raw/GC 30jun20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahoun\OneDrive\Desktop\Reservoir\Reservoirs\Data\DataNotYetUploadedToEDI\Raw_GHG\2020\Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\StreamTeam Analytical Lab\Projects\Carey Misc\Summer 2020 misc analyses\GC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0F8D27B-2910-46D0-8442-C50E37D3B651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBF3883-F1CE-400D-A6E9-E973B53A3B38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GC" sheetId="1" r:id="rId1"/>
@@ -477,24 +477,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:AU4"/>
+    <sheetView tabSelected="1" topLeftCell="AO3" workbookViewId="0">
+      <selection activeCell="AQ15" sqref="AQ15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" customWidth="1"/>
     <col min="30" max="30" width="22" customWidth="1"/>
-    <col min="37" max="37" width="10.33203125" customWidth="1"/>
+    <col min="37" max="37" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -505,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="3" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -630,7 +629,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>37</v>
       </c>
@@ -757,7 +756,7 @@
         <v>448.51521063946996</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>38</v>
       </c>
@@ -884,7 +883,7 @@
         <v>2038.66248264192</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>39</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>15374.386537670751</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1138,7 +1137,7 @@
         <v>11866.527673425631</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>41</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>14219.303918181231</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>42</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>10976.60963101068</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>43</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>1153.6485390610701</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>44</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>740.66266753712011</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>11505.29577400332</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>46</v>
       </c>
@@ -1900,7 +1899,7 @@
         <v>15473.947776926751</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>47</v>
       </c>
@@ -2027,7 +2026,7 @@
         <v>16164.858639614669</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>48</v>
       </c>
@@ -2154,7 +2153,7 @@
         <v>7040.5032356534703</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>49</v>
       </c>
@@ -2281,7 +2280,7 @@
         <v>7256.5842589920003</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>50</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>14164.707183045122</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>51</v>
       </c>
@@ -2535,7 +2534,7 @@
         <v>612.66697171199996</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>52</v>
       </c>

</xml_diff>